<commit_message>
* `request.options` in Excel is now aligned with API format; * Converter output is aligned with API format (intermediate representation for vrs-frontend is disabled)
</commit_message>
<xml_diff>
--- a/routing.flattened.xlsx
+++ b/routing.flattened.xlsx
@@ -1,24 +1,49 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28209"/>
+  <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/denis/demo/schema-tools/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Depots" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="Sites" state="visible" r:id="rId5"/>
-    <sheet sheetId="3" name="Fleet" state="visible" r:id="rId6"/>
-    <sheet sheetId="4" name="Options" state="visible" r:id="rId7"/>
-    <sheet sheetId="5" name="Constraints" state="visible" r:id="rId8"/>
-    <sheet sheetId="6" name="Depots legend" state="visible" r:id="rId9"/>
-    <sheet sheetId="7" name="Sites legend" state="visible" r:id="rId10"/>
-    <sheet sheetId="8" name="Fleet legend" state="visible" r:id="rId11"/>
-    <sheet sheetId="9" name="Options legend" state="visible" r:id="rId12"/>
-    <sheet sheetId="10" name="Constraints legend" state="visible" r:id="rId13"/>
+    <sheet name="Depots" sheetId="1" r:id="rId1"/>
+    <sheet name="Sites" sheetId="2" r:id="rId2"/>
+    <sheet name="Fleet" sheetId="3" r:id="rId3"/>
+    <sheet name="Options" sheetId="4" r:id="rId4"/>
+    <sheet name="Constraints" sheetId="5" r:id="rId5"/>
+    <sheet name="Depots legend" sheetId="6" r:id="rId6"/>
+    <sheet name="Sites legend" sheetId="7" r:id="rId7"/>
+    <sheet name="Fleet legend" sheetId="8" r:id="rId8"/>
+    <sheet name="Options legend" sheetId="9" r:id="rId9"/>
+    <sheet name="Constraints legend" sheetId="10" r:id="rId10"/>
   </sheets>
   <definedNames>
+    <definedName name="constraints_cols_default">'Constraints legend'!$E$2:$E$16</definedName>
+    <definedName name="constraints_cols_names">'Constraints legend'!$B$2:$B$16</definedName>
+    <definedName name="constraints_cols_required">'Constraints legend'!$D$2:$D$16</definedName>
+    <definedName name="constraints_cols_types">'Constraints legend'!$C$2:$C$16</definedName>
+    <definedName name="constraints.balanced_shifts.failure_costs.per_hour">'Constraints legend'!$B$6</definedName>
+    <definedName name="constraints.balanced_shifts.failure_costs.per_stop">'Constraints legend'!$B$7</definedName>
+    <definedName name="constraints.balanced_shifts.id">'Constraints legend'!$B$4</definedName>
+    <definedName name="constraints.employed_vehicles_limit.failure_costs.per_event">'Constraints legend'!$B$11</definedName>
+    <definedName name="constraints.employed_vehicles_limit.failure_costs.per_vehicle">'Constraints legend'!$B$12</definedName>
+    <definedName name="constraints.employed_vehicles_limit.min">'Constraints legend'!$B$9</definedName>
+    <definedName name="constraints.load_category_restrictions">'Constraints legend'!$B$2</definedName>
+    <definedName name="constraints.same_route_sites.failure_costs.per_site">'Constraints legend'!$B$16</definedName>
+    <definedName name="constraints.same_route_sites.id">'Constraints legend'!$B$14</definedName>
+    <definedName name="depots_cols_default">'Depots legend'!$E$2:$E$21</definedName>
+    <definedName name="depots_cols_names">'Depots legend'!$B$2:$B$21</definedName>
+    <definedName name="depots_cols_required">'Depots legend'!$D$2:$D$21</definedName>
+    <definedName name="depots_cols_types">'Depots legend'!$C$2:$C$21</definedName>
+    <definedName name="depots.delayed_start_costs.per_hour">'Depots legend'!$B$5</definedName>
+    <definedName name="depots.duration">'Depots legend'!$B$3</definedName>
     <definedName name="depots.id">'Depots legend'!$B$2</definedName>
-    <definedName name="depots.duration">'Depots legend'!$B$3</definedName>
-    <definedName name="depots.delayed_start_costs.per_hour">'Depots legend'!$B$5</definedName>
     <definedName name="depots.location.lat">'Depots legend'!$B$7</definedName>
     <definedName name="depots.location.lng">'Depots legend'!$B$8</definedName>
     <definedName name="depots.throughput_violation_costs.per_count">'Depots legend'!$B$11</definedName>
@@ -30,102 +55,155 @@
     <definedName name="depots.untimely_operations_costs.per_early_minute">'Depots legend'!$B$19</definedName>
     <definedName name="depots.untimely_operations_costs.per_event">'Depots legend'!$B$20</definedName>
     <definedName name="depots.untimely_operations_costs.per_late_minute">'Depots legend'!$B$21</definedName>
-    <definedName name="depots_cols_names">'Depots legend'!$B$2:$B$21</definedName>
-    <definedName name="depots_cols_types">'Depots legend'!$C$2:$C$21</definedName>
-    <definedName name="depots_cols_required">'Depots legend'!$D$2:$D$21</definedName>
-    <definedName name="depots_cols_default">'Depots legend'!$E$2:$E$21</definedName>
-    <definedName name="sites.id">'Sites legend'!$B$2</definedName>
-    <definedName name="sites.deliver_to">'Sites legend'!$B$3</definedName>
-    <definedName name="sites.duration">'Sites legend'!$B$4</definedName>
-    <definedName name="sites.job">'Sites legend'!$B$5</definedName>
-    <definedName name="sites.loading_duration">'Sites legend'!$B$6</definedName>
-    <definedName name="sites.preparing_duration">'Sites legend'!$B$7</definedName>
-    <definedName name="sites.required_capabilities">'Sites legend'!$B$8</definedName>
-    <definedName name="sites.same_route_key">'Sites legend'!$B$9</definedName>
-    <definedName name="sites.unperformed_cost">'Sites legend'!$B$10</definedName>
-    <definedName name="sites.load.categories">'Sites legend'!$B$12</definedName>
-    <definedName name="sites.load.count">'Sites legend'!$B$13</definedName>
-    <definedName name="sites.load.volume">'Sites legend'!$B$14</definedName>
-    <definedName name="sites.load.weight">'Sites legend'!$B$15</definedName>
-    <definedName name="sites.location.lat">'Sites legend'!$B$17</definedName>
-    <definedName name="sites.location.lng">'Sites legend'!$B$18</definedName>
-    <definedName name="sites.time_window.end">'Sites legend'!$B$20</definedName>
-    <definedName name="sites.time_window.start">'Sites legend'!$B$21</definedName>
-    <definedName name="sites.time_window.strict">'Sites legend'!$B$22</definedName>
-    <definedName name="sites.untimely_operations_costs.per_early_minute">'Sites legend'!$B$24</definedName>
-    <definedName name="sites.untimely_operations_costs.per_event">'Sites legend'!$B$25</definedName>
-    <definedName name="sites.untimely_operations_costs.per_late_minute">'Sites legend'!$B$26</definedName>
-    <definedName name="sites_cols_names">'Sites legend'!$B$2:$B$26</definedName>
-    <definedName name="sites_cols_types">'Sites legend'!$C$2:$C$26</definedName>
-    <definedName name="sites_cols_required">'Sites legend'!$D$2:$D$26</definedName>
-    <definedName name="sites_cols_default">'Sites legend'!$E$2:$E$26</definedName>
-    <definedName name="fleet.id">'Fleet legend'!$B$2</definedName>
+    <definedName name="fleet_cols_default">'Fleet legend'!$E$2:$E$50</definedName>
+    <definedName name="fleet_cols_names">'Fleet legend'!$B$2:$B$50</definedName>
+    <definedName name="fleet_cols_required">'Fleet legend'!$D$2:$D$50</definedName>
+    <definedName name="fleet_cols_types">'Fleet legend'!$C$2:$C$50</definedName>
     <definedName name="fleet.capabilities">'Fleet legend'!$B$3</definedName>
-    <definedName name="fleet.depot_id">'Fleet legend'!$B$4</definedName>
-    <definedName name="fleet.end_depot_id">'Fleet legend'!$B$5</definedName>
-    <definedName name="fleet.roundtrip">'Fleet legend'!$B$6</definedName>
     <definedName name="fleet.capacity.count">'Fleet legend'!$B$8</definedName>
     <definedName name="fleet.capacity.volume">'Fleet legend'!$B$9</definedName>
     <definedName name="fleet.capacity.weight">'Fleet legend'!$B$10</definedName>
+    <definedName name="fleet.costs.moved_load.per_countkm">'Fleet legend'!$B$19</definedName>
+    <definedName name="fleet.costs.moved_load.per_kgkm">'Fleet legend'!$B$18</definedName>
     <definedName name="fleet.costs.per_event">'Fleet legend'!$B$12</definedName>
     <definedName name="fleet.costs.per_hour">'Fleet legend'!$B$13</definedName>
     <definedName name="fleet.costs.per_km">'Fleet legend'!$B$14</definedName>
     <definedName name="fleet.costs.per_kwh">'Fleet legend'!$B$15</definedName>
     <definedName name="fleet.costs.per_site">'Fleet legend'!$B$16</definedName>
-    <definedName name="fleet.costs.moved_load.per_kgkm">'Fleet legend'!$B$18</definedName>
-    <definedName name="fleet.costs.moved_load.per_countkm">'Fleet legend'!$B$19</definedName>
+    <definedName name="fleet.depot_id">'Fleet legend'!$B$4</definedName>
+    <definedName name="fleet.end_depot_id">'Fleet legend'!$B$5</definedName>
+    <definedName name="fleet.id">'Fleet legend'!$B$2</definedName>
     <definedName name="fleet.min_load.count">'Fleet legend'!$B$21</definedName>
     <definedName name="fleet.min_load.volume">'Fleet legend'!$B$22</definedName>
     <definedName name="fleet.min_load.weight">'Fleet legend'!$B$23</definedName>
-    <definedName name="fleet.shifts.id">'Fleet legend'!$B$25</definedName>
+    <definedName name="fleet.roundtrip">'Fleet legend'!$B$6</definedName>
     <definedName name="fleet.shifts.balance_key">'Fleet legend'!$B$26</definedName>
-    <definedName name="fleet.shifts.duration_limit">'Fleet legend'!$B$27</definedName>
-    <definedName name="fleet.shifts.gap">'Fleet legend'!$B$28</definedName>
-    <definedName name="fleet.shifts.distance_limit.max">'Fleet legend'!$B$30</definedName>
     <definedName name="fleet.shifts.distance_limit.failure_costs.per_event">'Fleet legend'!$B$32</definedName>
     <definedName name="fleet.shifts.distance_limit.failure_costs.per_m">'Fleet legend'!$B$33</definedName>
-    <definedName name="fleet.shifts.energy_limit.max">'Fleet legend'!$B$35</definedName>
+    <definedName name="fleet.shifts.distance_limit.max">'Fleet legend'!$B$30</definedName>
+    <definedName name="fleet.shifts.duration_limit">'Fleet legend'!$B$27</definedName>
     <definedName name="fleet.shifts.energy_limit.failure_costs.per_event">'Fleet legend'!$B$37</definedName>
     <definedName name="fleet.shifts.energy_limit.failure_costs.per_kwh">'Fleet legend'!$B$38</definedName>
+    <definedName name="fleet.shifts.energy_limit.max">'Fleet legend'!$B$35</definedName>
+    <definedName name="fleet.shifts.gap">'Fleet legend'!$B$28</definedName>
+    <definedName name="fleet.shifts.id">'Fleet legend'!$B$25</definedName>
     <definedName name="fleet.shifts.late_operations_costs.per_event">'Fleet legend'!$B$40</definedName>
     <definedName name="fleet.shifts.late_operations_costs.per_late_minute">'Fleet legend'!$B$41</definedName>
-    <definedName name="fleet.shifts.stops_limit.min">'Fleet legend'!$B$43</definedName>
     <definedName name="fleet.shifts.stops_limit.failure_costs.per_event">'Fleet legend'!$B$45</definedName>
     <definedName name="fleet.shifts.stops_limit.failure_costs.per_stop">'Fleet legend'!$B$46</definedName>
+    <definedName name="fleet.shifts.stops_limit.min">'Fleet legend'!$B$43</definedName>
     <definedName name="fleet.shifts.time_window.end">'Fleet legend'!$B$48</definedName>
     <definedName name="fleet.shifts.time_window.start">'Fleet legend'!$B$49</definedName>
     <definedName name="fleet.shifts.time_window.strict">'Fleet legend'!$B$50</definedName>
-    <definedName name="fleet_cols_names">'Fleet legend'!$B$2:$B$50</definedName>
-    <definedName name="fleet_cols_types">'Fleet legend'!$C$2:$C$50</definedName>
-    <definedName name="fleet_cols_required">'Fleet legend'!$D$2:$D$50</definedName>
-    <definedName name="fleet_cols_default">'Fleet legend'!$E$2:$E$50</definedName>
+    <definedName name="options_cols_default">'Options legend'!$E$2:$E$5</definedName>
+    <definedName name="options_cols_names">'Options legend'!$B$2:$B$5</definedName>
+    <definedName name="options_cols_required">'Options legend'!$D$2:$D$5</definedName>
+    <definedName name="options_cols_types">'Options legend'!$C$2:$C$5</definedName>
     <definedName name="options.date">'Options legend'!$B$2</definedName>
     <definedName name="options.matrix">'Options legend'!$B$3</definedName>
     <definedName name="options.quality">'Options legend'!$B$4</definedName>
     <definedName name="options.timezone">'Options legend'!$B$5</definedName>
-    <definedName name="options_cols_names">'Options legend'!$B$2:$B$5</definedName>
-    <definedName name="options_cols_types">'Options legend'!$C$2:$C$5</definedName>
-    <definedName name="options_cols_required">'Options legend'!$D$2:$D$5</definedName>
-    <definedName name="options_cols_default">'Options legend'!$E$2:$E$5</definedName>
-    <definedName name="constraints.load_category_restrictions">'Constraints legend'!$B$2</definedName>
-    <definedName name="constraints.balanced_shifts.id">'Constraints legend'!$B$4</definedName>
-    <definedName name="constraints.balanced_shifts.failure_costs.per_hour">'Constraints legend'!$B$6</definedName>
-    <definedName name="constraints.balanced_shifts.failure_costs.per_stop">'Constraints legend'!$B$7</definedName>
-    <definedName name="constraints.employed_vehicles_limit.min">'Constraints legend'!$B$9</definedName>
-    <definedName name="constraints.employed_vehicles_limit.failure_costs.per_event">'Constraints legend'!$B$11</definedName>
-    <definedName name="constraints.employed_vehicles_limit.failure_costs.per_vehicle">'Constraints legend'!$B$12</definedName>
-    <definedName name="constraints.same_route_sites.id">'Constraints legend'!$B$14</definedName>
-    <definedName name="constraints.same_route_sites.failure_costs.per_site">'Constraints legend'!$B$16</definedName>
-    <definedName name="constraints_cols_names">'Constraints legend'!$B$2:$B$16</definedName>
-    <definedName name="constraints_cols_types">'Constraints legend'!$C$2:$C$16</definedName>
-    <definedName name="constraints_cols_required">'Constraints legend'!$D$2:$D$16</definedName>
-    <definedName name="constraints_cols_default">'Constraints legend'!$E$2:$E$16</definedName>
+    <definedName name="sites_cols_default">'Sites legend'!$E$2:$E$26</definedName>
+    <definedName name="sites_cols_names">'Sites legend'!$B$2:$B$26</definedName>
+    <definedName name="sites_cols_required">'Sites legend'!$D$2:$D$26</definedName>
+    <definedName name="sites_cols_types">'Sites legend'!$C$2:$C$26</definedName>
+    <definedName name="sites.deliver_to">'Sites legend'!$B$3</definedName>
+    <definedName name="sites.duration">'Sites legend'!$B$4</definedName>
+    <definedName name="sites.id">'Sites legend'!$B$2</definedName>
+    <definedName name="sites.job">'Sites legend'!$B$5</definedName>
+    <definedName name="sites.load.categories">'Sites legend'!$B$12</definedName>
+    <definedName name="sites.load.count">'Sites legend'!$B$13</definedName>
+    <definedName name="sites.load.volume">'Sites legend'!$B$14</definedName>
+    <definedName name="sites.load.weight">'Sites legend'!$B$15</definedName>
+    <definedName name="sites.loading_duration">'Sites legend'!$B$6</definedName>
+    <definedName name="sites.location.lat">'Sites legend'!$B$17</definedName>
+    <definedName name="sites.location.lng">'Sites legend'!$B$18</definedName>
+    <definedName name="sites.preparing_duration">'Sites legend'!$B$7</definedName>
+    <definedName name="sites.required_capabilities">'Sites legend'!$B$8</definedName>
+    <definedName name="sites.same_route_key">'Sites legend'!$B$9</definedName>
+    <definedName name="sites.time_window.end">'Sites legend'!$B$20</definedName>
+    <definedName name="sites.time_window.start">'Sites legend'!$B$21</definedName>
+    <definedName name="sites.time_window.strict">'Sites legend'!$B$22</definedName>
+    <definedName name="sites.unperformed_cost">'Sites legend'!$B$10</definedName>
+    <definedName name="sites.untimely_operations_costs.per_early_minute">'Sites legend'!$B$24</definedName>
+    <definedName name="sites.untimely_operations_costs.per_event">'Sites legend'!$B$25</definedName>
+    <definedName name="sites.untimely_operations_costs.per_late_minute">'Sites legend'!$B$26</definedName>
   </definedNames>
-  <calcPr calcId="171027" fullCalcOnLoad="1"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
-<file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="C9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Only one of possible options can be specified in the Excel sheet.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="C17" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Only one of possible options can be specified in the Excel sheet.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C24" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>List of values, represented as subtable with records in separate rows.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
@@ -134,6 +212,13 @@
     <comment ref="C3" authorId="0">
       <text>
         <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
           <t>List of values, represented as subtable with records in separate rows.</t>
         </r>
       </text>
@@ -141,47 +226,13 @@
     <comment ref="C13" authorId="0">
       <text>
         <r>
-          <t>List of values, represented as subtable with records in separate rows.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Author</author>
-  </authors>
-  <commentList>
-    <comment ref="C9" authorId="0">
-      <text>
-        <r>
-          <t>Only one of possible options can be specified in the Excel sheet.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Author</author>
-  </authors>
-  <commentList>
-    <comment ref="C17" authorId="0">
-      <text>
-        <r>
-          <t>Only one of possible options can be specified in the Excel sheet.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C24" authorId="0">
-      <text>
-        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
           <t>List of values, represented as subtable with records in separate rows.</t>
         </r>
       </text>
@@ -763,8 +814,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>vehicle.cost.per_hour</t>
@@ -910,8 +961,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>fleet{}.capacity</t>
@@ -925,8 +976,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>sites{}.load</t>
@@ -1151,8 +1202,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>hh</t>
@@ -1166,8 +1217,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>hh:mm</t>
@@ -1181,8 +1232,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>hh:mm:ss</t>
@@ -1219,8 +1270,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>1+</t>
@@ -1258,8 +1309,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>10:30:00</t>
@@ -1274,8 +1325,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>10:30</t>
@@ -1290,8 +1341,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>10</t>
@@ -1306,8 +1357,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>1+10:30</t>
@@ -1346,8 +1397,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>hh</t>
@@ -1361,8 +1412,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>hh:mm</t>
@@ -1376,8 +1427,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>hh:mm:ss</t>
@@ -1414,8 +1465,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>1+</t>
@@ -1453,8 +1504,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>10:30:00</t>
@@ -1469,8 +1520,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>10:30</t>
@@ -1485,8 +1536,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>10</t>
@@ -1501,8 +1552,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>1+10:30</t>
@@ -1707,8 +1758,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>pickup</t>
@@ -1722,8 +1773,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>id</t>
@@ -1849,8 +1900,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>delivery</t>
@@ -1880,8 +1931,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>pickup</t>
@@ -1895,8 +1946,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>deliver_to</t>
@@ -1961,8 +2012,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>depot.duration</t>
@@ -2104,8 +2155,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>fleet{}.capabilities</t>
@@ -2147,8 +2198,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>same_route_key</t>
@@ -2185,8 +2236,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>same_route_key</t>
@@ -2200,8 +2251,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>constraints.same_route_sites</t>
@@ -2347,8 +2398,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>weight</t>
@@ -2362,8 +2413,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>volume</t>
@@ -2428,8 +2479,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>volume</t>
@@ -2443,8 +2494,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>weight</t>
@@ -2458,8 +2509,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>weight</t>
@@ -2535,8 +2586,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>weight</t>
@@ -2550,8 +2601,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>volume</t>
@@ -2565,8 +2616,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>volume</t>
@@ -2766,8 +2817,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>depot_id</t>
@@ -2781,8 +2832,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>depots</t>
@@ -2796,8 +2847,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>depots</t>
@@ -2862,8 +2913,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>depot_id</t>
@@ -2877,8 +2928,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>depots</t>
@@ -2943,8 +2994,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>roundtrip</t>
@@ -2958,8 +3009,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>false</t>
@@ -3207,8 +3258,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>per_kwh</t>
@@ -3222,8 +3273,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>energy</t>
@@ -3590,8 +3641,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>constraints.balanced_shifts</t>
@@ -3646,8 +3697,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>late_operations_costs</t>
@@ -3712,8 +3763,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>gap</t>
@@ -3778,8 +3829,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>distance_limit.failure_costs</t>
@@ -3849,8 +3900,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>distance_limit.max</t>
@@ -3971,8 +4022,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>energy_limit.failure_costs</t>
@@ -4042,8 +4093,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>energy_limit.max</t>
@@ -4139,8 +4190,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>time_window.strict = true</t>
@@ -4292,8 +4343,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>stops_limit.min</t>
@@ -4437,8 +4488,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>yyyy-MM-dd</t>
@@ -4476,8 +4527,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>2020-09-01</t>
@@ -4525,8 +4576,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>here</t>
@@ -4541,8 +4592,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>osrm</t>
@@ -4620,8 +4671,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>debug</t>
@@ -4651,8 +4702,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>normal</t>
@@ -4682,8 +4733,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>high</t>
@@ -4749,8 +4800,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>UTC</t>
@@ -4765,8 +4816,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>UTC+5</t>
@@ -4781,8 +4832,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>Europe/Berlin</t>
@@ -4797,8 +4848,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>Asia/Dubai</t>
@@ -4813,8 +4864,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>America/Los_Angeles</t>
@@ -4872,8 +4923,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>sites{}.load.category</t>
@@ -4961,8 +5012,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>fleet{}.shifts{}.balancing_key</t>
@@ -5310,8 +5361,8 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
         <color rgb="FF3355FF"/>
-        <sz val="12"/>
         <rFont val="Courier"/>
       </rPr>
       <t>sites{}.same_route_key</t>
@@ -5382,14 +5433,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <b/>
@@ -5402,15 +5453,15 @@
     </font>
     <font>
       <i/>
+      <sz val="10"/>
       <color rgb="FF555555"/>
-      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
       <i/>
       <u/>
+      <sz val="10"/>
       <color rgb="FF3355FF"/>
-      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -5418,8 +5469,8 @@
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="12"/>
       <color rgb="FF3355FF"/>
-      <sz val="12"/>
       <name val="Courier"/>
     </font>
   </fonts>
@@ -5460,10 +5511,10 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="bottom"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="bottom"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -5830,12 +5881,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" style="1" customWidth="1"/>
     <col min="2" max="3" width="14" style="1" customWidth="1"/>
@@ -5845,24 +5896,21 @@
     <col min="7" max="7" width="17" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
       <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" ht="25" customHeight="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="2" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -5885,75 +5933,75 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" ht="12.5" customHeight="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="4" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="str">
-        <f>INDEX(depots_cols_types, MATCH(A2, depots_cols_names, 0)) &amp; IF("Required" = INDEX(depots_cols_required, MATCH(A2, depots_cols_names, 0)), "*", " (" &amp; INDEX(depots_cols_default, MATCH(A2, depots_cols_names, 0)) &amp; ")")</f>
-        <v>(recalculate)</v>
+        <f t="shared" ref="A3:G3" si="0">INDEX(depots_cols_types, MATCH(A2, depots_cols_names, 0)) &amp; IF("Required" = INDEX(depots_cols_required, MATCH(A2, depots_cols_names, 0)), "*", " (" &amp; INDEX(depots_cols_default, MATCH(A2, depots_cols_names, 0)) &amp; ")")</f>
+        <v>string*</v>
       </c>
       <c r="B3" s="5" t="str">
-        <f>INDEX(depots_cols_types, MATCH(B2, depots_cols_names, 0)) &amp; IF("Required" = INDEX(depots_cols_required, MATCH(B2, depots_cols_names, 0)), "*", " (" &amp; INDEX(depots_cols_default, MATCH(B2, depots_cols_names, 0)) &amp; ")")</f>
-        <v>(recalculate)</v>
+        <f t="shared" si="0"/>
+        <v>number*</v>
       </c>
       <c r="C3" s="5" t="str">
-        <f>INDEX(depots_cols_types, MATCH(C2, depots_cols_names, 0)) &amp; IF("Required" = INDEX(depots_cols_required, MATCH(C2, depots_cols_names, 0)), "*", " (" &amp; INDEX(depots_cols_default, MATCH(C2, depots_cols_names, 0)) &amp; ")")</f>
-        <v>(recalculate)</v>
+        <f t="shared" si="0"/>
+        <v>number*</v>
       </c>
       <c r="D3" s="5" t="str">
-        <f>INDEX(depots_cols_types, MATCH(D2, depots_cols_names, 0)) &amp; IF("Required" = INDEX(depots_cols_required, MATCH(D2, depots_cols_names, 0)), "*", " (" &amp; INDEX(depots_cols_default, MATCH(D2, depots_cols_names, 0)) &amp; ")")</f>
-        <v>(recalculate)</v>
+        <f t="shared" si="0"/>
+        <v>string*</v>
       </c>
       <c r="E3" s="5" t="str">
-        <f>INDEX(depots_cols_types, MATCH(E2, depots_cols_names, 0)) &amp; IF("Required" = INDEX(depots_cols_required, MATCH(E2, depots_cols_names, 0)), "*", " (" &amp; INDEX(depots_cols_default, MATCH(E2, depots_cols_names, 0)) &amp; ")")</f>
-        <v>(recalculate)</v>
+        <f t="shared" si="0"/>
+        <v>string*</v>
       </c>
       <c r="F3" s="5" t="str">
-        <f>INDEX(depots_cols_types, MATCH(F2, depots_cols_names, 0)) &amp; IF("Required" = INDEX(depots_cols_required, MATCH(F2, depots_cols_names, 0)), "*", " (" &amp; INDEX(depots_cols_default, MATCH(F2, depots_cols_names, 0)) &amp; ")")</f>
-        <v>(recalculate)</v>
+        <f t="shared" si="0"/>
+        <v>boolean (FALSE)</v>
       </c>
       <c r="G3" s="5" t="str">
-        <f>INDEX(depots_cols_types, MATCH(G2, depots_cols_names, 0)) &amp; IF("Required" = INDEX(depots_cols_required, MATCH(G2, depots_cols_names, 0)), "*", " (" &amp; INDEX(depots_cols_default, MATCH(G2, depots_cols_names, 0)) &amp; ")")</f>
-        <v>(recalculate)</v>
-      </c>
-    </row>
-    <row r="4" ht="20" customHeight="1" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>number (0)</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="str">
-        <f>HYPERLINK("#depots." &amp; A2, "help")</f>
-        <v>(recalculate)</v>
+        <f t="shared" ref="A4:G4" si="1">HYPERLINK("#depots." &amp; A2, "help")</f>
+        <v>help</v>
       </c>
       <c r="B4" s="7" t="str">
-        <f>HYPERLINK("#depots." &amp; B2, "help")</f>
-        <v>(recalculate)</v>
+        <f t="shared" si="1"/>
+        <v>help</v>
       </c>
       <c r="C4" s="7" t="str">
-        <f>HYPERLINK("#depots." &amp; C2, "help")</f>
-        <v>(recalculate)</v>
+        <f t="shared" si="1"/>
+        <v>help</v>
       </c>
       <c r="D4" s="7" t="str">
-        <f>HYPERLINK("#depots." &amp; D2, "help")</f>
-        <v>(recalculate)</v>
+        <f t="shared" si="1"/>
+        <v>help</v>
       </c>
       <c r="E4" s="7" t="str">
-        <f>HYPERLINK("#depots." &amp; E2, "help")</f>
-        <v>(recalculate)</v>
+        <f t="shared" si="1"/>
+        <v>help</v>
       </c>
       <c r="F4" s="7" t="str">
-        <f>HYPERLINK("#depots." &amp; F2, "help")</f>
-        <v>(recalculate)</v>
+        <f t="shared" si="1"/>
+        <v>help</v>
       </c>
       <c r="G4" s="7" t="str">
-        <f>HYPERLINK("#depots." &amp; G2, "help")</f>
-        <v>(recalculate)</v>
-      </c>
-    </row>
-    <row r="5" ht="25" customHeight="1" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>help</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="8">
-        <v>52.524373</v>
+        <v>52.524372999999997</v>
       </c>
       <c r="C5" s="8">
-        <v>13.141106</v>
+        <v>13.141106000000001</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>12</v>
@@ -5968,7 +6016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" ht="25" customHeight="1" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>14</v>
       </c>
@@ -5998,20 +6046,20 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" style="9" customWidth="1"/>
     <col min="2" max="2" width="50" style="9" customWidth="1"/>
@@ -6021,7 +6069,7 @@
     <col min="6" max="6" width="64" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="25" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>132</v>
       </c>
@@ -6041,7 +6089,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="10" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="B2" s="10" t="s">
         <v>127</v>
       </c>
@@ -6058,7 +6106,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="9" customFormat="1" ht="160" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>283</v>
       </c>
@@ -6074,7 +6122,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="4" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" s="10" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B4" s="10" t="s">
         <v>128</v>
       </c>
@@ -6091,7 +6139,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" s="9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>285</v>
       </c>
@@ -6107,7 +6155,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="6" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" s="10" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="B6" s="10" t="s">
         <v>129</v>
       </c>
@@ -6124,7 +6172,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="7" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" s="10" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="B7" s="10" t="s">
         <v>288</v>
       </c>
@@ -6141,7 +6189,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" s="9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>290</v>
       </c>
@@ -6157,7 +6205,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="9" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" s="10" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B9" s="10" t="s">
         <v>292</v>
       </c>
@@ -6174,7 +6222,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" s="9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>294</v>
       </c>
@@ -6190,7 +6238,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="11" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" s="10" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B11" s="10" t="s">
         <v>296</v>
       </c>
@@ -6207,7 +6255,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="12" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" s="10" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B12" s="10" t="s">
         <v>298</v>
       </c>
@@ -6224,7 +6272,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" s="9" customFormat="1" ht="144" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
         <v>300</v>
       </c>
@@ -6240,7 +6288,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="14" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" s="10" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B14" s="10" t="s">
         <v>130</v>
       </c>
@@ -6257,7 +6305,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" s="9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
         <v>302</v>
       </c>
@@ -6273,7 +6321,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="16" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" s="10" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B16" s="10" t="s">
         <v>131</v>
       </c>
@@ -6292,8 +6340,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6303,10 +6351,10 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" style="1" customWidth="1"/>
     <col min="2" max="3" width="14" style="1" customWidth="1"/>
@@ -6319,19 +6367,16 @@
     <col min="10" max="10" width="22" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="25" customHeight="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="1"/>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
       <c r="G1" s="1" t="s">
         <v>17</v>
       </c>
@@ -6345,7 +6390,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" ht="25" customHeight="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="2" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -6377,99 +6422,99 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" ht="12.5" customHeight="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" s="4" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="str">
-        <f>INDEX(sites_cols_types, MATCH(A2, sites_cols_names, 0)) &amp; IF("Required" = INDEX(sites_cols_required, MATCH(A2, sites_cols_names, 0)), "*", " (" &amp; INDEX(sites_cols_default, MATCH(A2, sites_cols_names, 0)) &amp; ")")</f>
-        <v>(recalculate)</v>
+        <f t="shared" ref="A3:J3" si="0">INDEX(sites_cols_types, MATCH(A2, sites_cols_names, 0)) &amp; IF("Required" = INDEX(sites_cols_required, MATCH(A2, sites_cols_names, 0)), "*", " (" &amp; INDEX(sites_cols_default, MATCH(A2, sites_cols_names, 0)) &amp; ")")</f>
+        <v>string*</v>
       </c>
       <c r="B3" s="5" t="str">
-        <f>INDEX(sites_cols_types, MATCH(B2, sites_cols_names, 0)) &amp; IF("Required" = INDEX(sites_cols_required, MATCH(B2, sites_cols_names, 0)), "*", " (" &amp; INDEX(sites_cols_default, MATCH(B2, sites_cols_names, 0)) &amp; ")")</f>
-        <v>(recalculate)</v>
+        <f t="shared" si="0"/>
+        <v>number*</v>
       </c>
       <c r="C3" s="5" t="str">
-        <f>INDEX(sites_cols_types, MATCH(C2, sites_cols_names, 0)) &amp; IF("Required" = INDEX(sites_cols_required, MATCH(C2, sites_cols_names, 0)), "*", " (" &amp; INDEX(sites_cols_default, MATCH(C2, sites_cols_names, 0)) &amp; ")")</f>
-        <v>(recalculate)</v>
+        <f t="shared" si="0"/>
+        <v>number*</v>
       </c>
       <c r="D3" s="5" t="str">
-        <f>INDEX(sites_cols_types, MATCH(D2, sites_cols_names, 0)) &amp; IF("Required" = INDEX(sites_cols_required, MATCH(D2, sites_cols_names, 0)), "*", " (" &amp; INDEX(sites_cols_default, MATCH(D2, sites_cols_names, 0)) &amp; ")")</f>
-        <v>(recalculate)</v>
+        <f t="shared" si="0"/>
+        <v>string*</v>
       </c>
       <c r="E3" s="5" t="str">
-        <f>INDEX(sites_cols_types, MATCH(E2, sites_cols_names, 0)) &amp; IF("Required" = INDEX(sites_cols_required, MATCH(E2, sites_cols_names, 0)), "*", " (" &amp; INDEX(sites_cols_default, MATCH(E2, sites_cols_names, 0)) &amp; ")")</f>
-        <v>(recalculate)</v>
+        <f t="shared" si="0"/>
+        <v>string*</v>
       </c>
       <c r="F3" s="5" t="str">
-        <f>INDEX(sites_cols_types, MATCH(F2, sites_cols_names, 0)) &amp; IF("Required" = INDEX(sites_cols_required, MATCH(F2, sites_cols_names, 0)), "*", " (" &amp; INDEX(sites_cols_default, MATCH(F2, sites_cols_names, 0)) &amp; ")")</f>
-        <v>(recalculate)</v>
+        <f t="shared" si="0"/>
+        <v>boolean (FALSE)</v>
       </c>
       <c r="G3" s="5" t="str">
-        <f>INDEX(sites_cols_types, MATCH(G2, sites_cols_names, 0)) &amp; IF("Required" = INDEX(sites_cols_required, MATCH(G2, sites_cols_names, 0)), "*", " (" &amp; INDEX(sites_cols_default, MATCH(G2, sites_cols_names, 0)) &amp; ")")</f>
-        <v>(recalculate)</v>
+        <f t="shared" si="0"/>
+        <v>number (0)</v>
       </c>
       <c r="H3" s="5" t="str">
-        <f>INDEX(sites_cols_types, MATCH(H2, sites_cols_names, 0)) &amp; IF("Required" = INDEX(sites_cols_required, MATCH(H2, sites_cols_names, 0)), "*", " (" &amp; INDEX(sites_cols_default, MATCH(H2, sites_cols_names, 0)) &amp; ")")</f>
-        <v>(recalculate)</v>
+        <f t="shared" si="0"/>
+        <v>string (delivery)</v>
       </c>
       <c r="I3" s="5" t="str">
-        <f>INDEX(sites_cols_types, MATCH(I2, sites_cols_names, 0)) &amp; IF("Required" = INDEX(sites_cols_required, MATCH(I2, sites_cols_names, 0)), "*", " (" &amp; INDEX(sites_cols_default, MATCH(I2, sites_cols_names, 0)) &amp; ")")</f>
-        <v>(recalculate)</v>
+        <f t="shared" si="0"/>
+        <v>number (0)</v>
       </c>
       <c r="J3" s="5" t="str">
-        <f>INDEX(sites_cols_types, MATCH(J2, sites_cols_names, 0)) &amp; IF("Required" = INDEX(sites_cols_required, MATCH(J2, sites_cols_names, 0)), "*", " (" &amp; INDEX(sites_cols_default, MATCH(J2, sites_cols_names, 0)) &amp; ")")</f>
-        <v>(recalculate)</v>
-      </c>
-    </row>
-    <row r="4" ht="20" customHeight="1" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>number (100000000)</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="str">
-        <f>HYPERLINK("#sites." &amp; A2, "help")</f>
-        <v>(recalculate)</v>
+        <f t="shared" ref="A4:J4" si="1">HYPERLINK("#sites." &amp; A2, "help")</f>
+        <v>help</v>
       </c>
       <c r="B4" s="7" t="str">
-        <f>HYPERLINK("#sites." &amp; B2, "help")</f>
-        <v>(recalculate)</v>
+        <f t="shared" si="1"/>
+        <v>help</v>
       </c>
       <c r="C4" s="7" t="str">
-        <f>HYPERLINK("#sites." &amp; C2, "help")</f>
-        <v>(recalculate)</v>
+        <f t="shared" si="1"/>
+        <v>help</v>
       </c>
       <c r="D4" s="7" t="str">
-        <f>HYPERLINK("#sites." &amp; D2, "help")</f>
-        <v>(recalculate)</v>
+        <f t="shared" si="1"/>
+        <v>help</v>
       </c>
       <c r="E4" s="7" t="str">
-        <f>HYPERLINK("#sites." &amp; E2, "help")</f>
-        <v>(recalculate)</v>
+        <f t="shared" si="1"/>
+        <v>help</v>
       </c>
       <c r="F4" s="7" t="str">
-        <f>HYPERLINK("#sites." &amp; F2, "help")</f>
-        <v>(recalculate)</v>
+        <f t="shared" si="1"/>
+        <v>help</v>
       </c>
       <c r="G4" s="7" t="str">
-        <f>HYPERLINK("#sites." &amp; G2, "help")</f>
-        <v>(recalculate)</v>
+        <f t="shared" si="1"/>
+        <v>help</v>
       </c>
       <c r="H4" s="7" t="str">
-        <f>HYPERLINK("#sites." &amp; H2, "help")</f>
-        <v>(recalculate)</v>
+        <f t="shared" si="1"/>
+        <v>help</v>
       </c>
       <c r="I4" s="7" t="str">
-        <f>HYPERLINK("#sites." &amp; I2, "help")</f>
-        <v>(recalculate)</v>
+        <f t="shared" si="1"/>
+        <v>help</v>
       </c>
       <c r="J4" s="7" t="str">
-        <f>HYPERLINK("#sites." &amp; J2, "help")</f>
-        <v>(recalculate)</v>
-      </c>
-    </row>
-    <row r="5" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>help</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="8">
-        <v>52.4326111</v>
+        <v>52.432611100000003</v>
       </c>
       <c r="C5" s="8">
-        <v>13.3000801</v>
+        <v>13.300080100000001</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>25</v>
@@ -6493,15 +6538,15 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="6" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="8">
-        <v>52.5212442</v>
+        <v>52.521244199999998</v>
       </c>
       <c r="C6" s="8">
-        <v>13.409629</v>
+        <v>13.409629000000001</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>26</v>
@@ -6525,12 +6570,12 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="7" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>30</v>
       </c>
       <c r="B7" s="8">
-        <v>52.5062211</v>
+        <v>52.506221099999998</v>
       </c>
       <c r="C7" s="8">
         <v>13.294257</v>
@@ -6557,12 +6602,12 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="8" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>33</v>
       </c>
       <c r="B8" s="8">
-        <v>52.4846191</v>
+        <v>52.484619100000003</v>
       </c>
       <c r="C8" s="8">
         <v>13.6281143</v>
@@ -6589,12 +6634,12 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>36</v>
       </c>
       <c r="B9" s="8">
-        <v>52.5179061</v>
+        <v>52.517906099999998</v>
       </c>
       <c r="C9" s="8">
         <v>13.3878263</v>
@@ -6621,12 +6666,12 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="10" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>37</v>
       </c>
       <c r="B10" s="8">
-        <v>52.4111088</v>
+        <v>52.411108800000001</v>
       </c>
       <c r="C10" s="8">
         <v>13.3777211</v>
@@ -6653,12 +6698,12 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="11" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>38</v>
       </c>
       <c r="B11" s="8">
-        <v>52.5124786</v>
+        <v>52.512478600000001</v>
       </c>
       <c r="C11" s="8">
         <v>13.4571679</v>
@@ -6685,15 +6730,15 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="12" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>39</v>
       </c>
       <c r="B12" s="8">
-        <v>52.523965</v>
+        <v>52.523964999999997</v>
       </c>
       <c r="C12" s="8">
-        <v>13.3974459</v>
+        <v>13.397445899999999</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>34</v>
@@ -6717,12 +6762,12 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="13" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>40</v>
       </c>
       <c r="B13" s="8">
-        <v>52.4505702</v>
+        <v>52.450570200000001</v>
       </c>
       <c r="C13" s="8">
         <v>13.3215021</v>
@@ -6749,7 +6794,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="14" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>42</v>
       </c>
@@ -6781,15 +6826,15 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="15" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>43</v>
       </c>
       <c r="B15" s="8">
-        <v>52.5395739</v>
+        <v>52.539573900000001</v>
       </c>
       <c r="C15" s="8">
-        <v>13.406498</v>
+        <v>13.406497999999999</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>35</v>
@@ -6813,7 +6858,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="16" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>45</v>
       </c>
@@ -6821,7 +6866,7 @@
         <v>52.5398383</v>
       </c>
       <c r="C16" s="8">
-        <v>13.4068458</v>
+        <v>13.406845799999999</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>34</v>
@@ -6845,12 +6890,12 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="17" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
         <v>46</v>
       </c>
       <c r="B17" s="8">
-        <v>52.4941864</v>
+        <v>52.494186399999997</v>
       </c>
       <c r="C17" s="8">
         <v>13.331275</v>
@@ -6877,15 +6922,15 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="18" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
         <v>47</v>
       </c>
       <c r="B18" s="8">
-        <v>52.4939677</v>
+        <v>52.493967699999999</v>
       </c>
       <c r="C18" s="8">
-        <v>13.3539664</v>
+        <v>13.353966399999999</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>31</v>
@@ -6909,12 +6954,12 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="19" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
         <v>48</v>
       </c>
       <c r="B19" s="8">
-        <v>52.529452</v>
+        <v>52.529451999999999</v>
       </c>
       <c r="C19" s="8">
         <v>13.400719</v>
@@ -6941,12 +6986,12 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="20" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
         <v>50</v>
       </c>
       <c r="B20" s="8">
-        <v>52.4574255</v>
+        <v>52.457425499999999</v>
       </c>
       <c r="C20" s="8">
         <v>13.533528</v>
@@ -6973,7 +7018,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="21" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
         <v>51</v>
       </c>
@@ -7005,12 +7050,12 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="22" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
         <v>52</v>
       </c>
       <c r="B22" s="8">
-        <v>52.4348924</v>
+        <v>52.434892400000003</v>
       </c>
       <c r="C22" s="8">
         <v>13.3786126</v>
@@ -7037,15 +7082,15 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="23" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>53</v>
       </c>
       <c r="B23" s="8">
-        <v>52.4955155</v>
+        <v>52.495515500000003</v>
       </c>
       <c r="C23" s="8">
-        <v>13.3428785</v>
+        <v>13.342878499999999</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>26</v>
@@ -7069,15 +7114,15 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="24" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
         <v>54</v>
       </c>
       <c r="B24" s="8">
-        <v>52.4940664</v>
+        <v>52.494066400000001</v>
       </c>
       <c r="C24" s="8">
-        <v>13.3965214</v>
+        <v>13.396521399999999</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>25</v>
@@ -7101,12 +7146,12 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="25" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
         <v>55</v>
       </c>
       <c r="B25" s="8">
-        <v>52.4086369</v>
+        <v>52.408636899999998</v>
       </c>
       <c r="C25" s="8">
         <v>13.5824034</v>
@@ -7133,12 +7178,12 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="26" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
         <v>56</v>
       </c>
       <c r="B26" s="8">
-        <v>52.522074</v>
+        <v>52.522074000000003</v>
       </c>
       <c r="C26" s="8">
         <v>13.3361319</v>
@@ -7165,12 +7210,12 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="27" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
         <v>57</v>
       </c>
       <c r="B27" s="8">
-        <v>52.5481127</v>
+        <v>52.548112699999997</v>
       </c>
       <c r="C27" s="8">
         <v>13.4130983</v>
@@ -7197,12 +7242,12 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="28" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
         <v>58</v>
       </c>
       <c r="B28" s="8">
-        <v>52.5271371</v>
+        <v>52.527137099999997</v>
       </c>
       <c r="C28" s="8">
         <v>13.385754</v>
@@ -7229,12 +7274,12 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="29" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
         <v>59</v>
       </c>
       <c r="B29" s="8">
-        <v>52.4410887</v>
+        <v>52.441088700000002</v>
       </c>
       <c r="C29" s="8">
         <v>13.2438526</v>
@@ -7261,12 +7306,12 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="30" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
         <v>60</v>
       </c>
       <c r="B30" s="8">
-        <v>52.5216052</v>
+        <v>52.521605200000003</v>
       </c>
       <c r="C30" s="8">
         <v>13.1651872</v>
@@ -7293,12 +7338,12 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="31" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
         <v>61</v>
       </c>
       <c r="B31" s="8">
-        <v>52.5272355</v>
+        <v>52.527235500000003</v>
       </c>
       <c r="C31" s="8">
         <v>13.3886032</v>
@@ -7325,12 +7370,12 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="32" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
         <v>62</v>
       </c>
       <c r="B32" s="8">
-        <v>52.5698918</v>
+        <v>52.569891800000001</v>
       </c>
       <c r="C32" s="8">
         <v>13.495771</v>
@@ -7357,12 +7402,12 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="33" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
         <v>63</v>
       </c>
       <c r="B33" s="8">
-        <v>52.5283329</v>
+        <v>52.528332900000002</v>
       </c>
       <c r="C33" s="8">
         <v>13.3939457</v>
@@ -7389,7 +7434,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="34" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
         <v>64</v>
       </c>
@@ -7421,7 +7466,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="35" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
         <v>65</v>
       </c>
@@ -7453,12 +7498,12 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="36" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
         <v>66</v>
       </c>
       <c r="B36" s="8">
-        <v>52.5244858</v>
+        <v>52.524485800000001</v>
       </c>
       <c r="C36" s="8">
         <v>13.3301178</v>
@@ -7485,12 +7530,12 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="37" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
         <v>67</v>
       </c>
       <c r="B37" s="8">
-        <v>52.5518746</v>
+        <v>52.551874599999998</v>
       </c>
       <c r="C37" s="8">
         <v>13.3554694</v>
@@ -7517,12 +7562,12 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="38" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
         <v>68</v>
       </c>
       <c r="B38" s="8">
-        <v>52.4565312</v>
+        <v>52.456531200000001</v>
       </c>
       <c r="C38" s="8">
         <v>13.5105881</v>
@@ -7549,15 +7594,15 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="39" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="8" t="s">
         <v>69</v>
       </c>
       <c r="B39" s="8">
-        <v>52.4977937</v>
+        <v>52.497793700000003</v>
       </c>
       <c r="C39" s="8">
-        <v>13.3246353</v>
+        <v>13.324635300000001</v>
       </c>
       <c r="D39" s="8" t="s">
         <v>26</v>
@@ -7581,15 +7626,15 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="40" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="8" t="s">
         <v>70</v>
       </c>
       <c r="B40" s="8">
-        <v>52.5475361</v>
+        <v>52.547536100000002</v>
       </c>
       <c r="C40" s="8">
-        <v>13.3689039</v>
+        <v>13.368903899999999</v>
       </c>
       <c r="D40" s="8" t="s">
         <v>34</v>
@@ -7613,15 +7658,15 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="41" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="8" t="s">
         <v>71</v>
       </c>
       <c r="B41" s="8">
-        <v>52.4555158</v>
+        <v>52.455515800000001</v>
       </c>
       <c r="C41" s="8">
-        <v>13.5771852</v>
+        <v>13.577185200000001</v>
       </c>
       <c r="D41" s="8" t="s">
         <v>35</v>
@@ -7645,12 +7690,12 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="42" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="8" t="s">
         <v>72</v>
       </c>
       <c r="B42" s="8">
-        <v>52.5280441</v>
+        <v>52.528044100000002</v>
       </c>
       <c r="C42" s="8">
         <v>13.3289036</v>
@@ -7677,12 +7722,12 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="43" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="8" t="s">
         <v>73</v>
       </c>
       <c r="B43" s="8">
-        <v>52.496232</v>
+        <v>52.496231999999999</v>
       </c>
       <c r="C43" s="8">
         <v>13.295239</v>
@@ -7709,7 +7754,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="44" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
         <v>74</v>
       </c>
@@ -7741,12 +7786,12 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="45" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="8" t="s">
         <v>75</v>
       </c>
       <c r="B45" s="8">
-        <v>52.5226824</v>
+        <v>52.522682400000001</v>
       </c>
       <c r="C45" s="8">
         <v>13.3490454</v>
@@ -7773,15 +7818,15 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="46" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="8" t="s">
         <v>76</v>
       </c>
       <c r="B46" s="8">
-        <v>52.4235698</v>
+        <v>52.423569800000003</v>
       </c>
       <c r="C46" s="8">
-        <v>13.3181763</v>
+        <v>13.318176299999999</v>
       </c>
       <c r="D46" s="8" t="s">
         <v>31</v>
@@ -7805,12 +7850,12 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="47" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="8" t="s">
         <v>77</v>
       </c>
       <c r="B47" s="8">
-        <v>52.4930783</v>
+        <v>52.493078300000001</v>
       </c>
       <c r="C47" s="8">
         <v>13.3473845</v>
@@ -7837,12 +7882,12 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="48" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="8" t="s">
         <v>78</v>
       </c>
       <c r="B48" s="8">
-        <v>52.5075921</v>
+        <v>52.507592099999997</v>
       </c>
       <c r="C48" s="8">
         <v>13.3199919</v>
@@ -7869,15 +7914,15 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="49" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="8" t="s">
         <v>79</v>
       </c>
       <c r="B49" s="8">
-        <v>52.4287929</v>
+        <v>52.428792899999998</v>
       </c>
       <c r="C49" s="8">
-        <v>13.3278647</v>
+        <v>13.327864699999999</v>
       </c>
       <c r="D49" s="8" t="s">
         <v>34</v>
@@ -7901,7 +7946,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="50" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="8" t="s">
         <v>80</v>
       </c>
@@ -7909,7 +7954,7 @@
         <v>52.4914931</v>
       </c>
       <c r="C50" s="8">
-        <v>13.4136359</v>
+        <v>13.413635899999999</v>
       </c>
       <c r="D50" s="8" t="s">
         <v>31</v>
@@ -7933,12 +7978,12 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="51" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="8" t="s">
         <v>81</v>
       </c>
       <c r="B51" s="8">
-        <v>52.4620066</v>
+        <v>52.462006600000002</v>
       </c>
       <c r="C51" s="8">
         <v>13.3187993</v>
@@ -7965,12 +8010,12 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="52" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="8" t="s">
         <v>82</v>
       </c>
       <c r="B52" s="8">
-        <v>52.5121223</v>
+        <v>52.512122300000001</v>
       </c>
       <c r="C52" s="8">
         <v>13.37829</v>
@@ -7997,15 +8042,15 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="53" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="8" t="s">
         <v>83</v>
       </c>
       <c r="B53" s="8">
-        <v>52.5273922</v>
+        <v>52.527392200000001</v>
       </c>
       <c r="C53" s="8">
-        <v>13.4024727</v>
+        <v>13.402472700000001</v>
       </c>
       <c r="D53" s="8" t="s">
         <v>31</v>
@@ -8029,12 +8074,12 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="54" ht="25" customHeight="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="8" t="s">
         <v>84</v>
       </c>
       <c r="B54" s="8">
-        <v>52.5077516</v>
+        <v>52.507751599999999</v>
       </c>
       <c r="C54" s="8">
         <v>13.4206012</v>
@@ -8068,7 +8113,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
 
@@ -8078,10 +8123,10 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" style="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="1" customWidth="1"/>
@@ -8096,7 +8141,7 @@
     <col min="11" max="11" width="16" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="25" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>85</v>
       </c>
@@ -8112,8 +8157,6 @@
       <c r="E1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
       <c r="H1" s="1" t="s">
         <v>89</v>
       </c>
@@ -8127,7 +8170,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" ht="25" customHeight="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="2" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -8162,99 +8205,99 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" ht="12.5" customHeight="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="4" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="str">
-        <f>INDEX(fleet_cols_types, MATCH(A2, fleet_cols_names, 0)) &amp; IF("Required" = INDEX(fleet_cols_required, MATCH(A2, fleet_cols_names, 0)), "*", " (" &amp; INDEX(fleet_cols_default, MATCH(A2, fleet_cols_names, 0)) &amp; ")")</f>
-        <v>(recalculate)</v>
+        <f t="shared" ref="A3:K3" si="0">INDEX(fleet_cols_types, MATCH(A2, fleet_cols_names, 0)) &amp; IF("Required" = INDEX(fleet_cols_required, MATCH(A2, fleet_cols_names, 0)), "*", " (" &amp; INDEX(fleet_cols_default, MATCH(A2, fleet_cols_names, 0)) &amp; ")")</f>
+        <v>string*</v>
       </c>
       <c r="B3" s="5" t="str">
-        <f>INDEX(fleet_cols_types, MATCH(B2, fleet_cols_names, 0)) &amp; IF("Required" = INDEX(fleet_cols_required, MATCH(B2, fleet_cols_names, 0)), "*", " (" &amp; INDEX(fleet_cols_default, MATCH(B2, fleet_cols_names, 0)) &amp; ")")</f>
-        <v>(recalculate)</v>
+        <f t="shared" si="0"/>
+        <v>string ()</v>
       </c>
       <c r="C3" s="5" t="str">
-        <f>INDEX(fleet_cols_types, MATCH(C2, fleet_cols_names, 0)) &amp; IF("Required" = INDEX(fleet_cols_required, MATCH(C2, fleet_cols_names, 0)), "*", " (" &amp; INDEX(fleet_cols_default, MATCH(C2, fleet_cols_names, 0)) &amp; ")")</f>
-        <v>(recalculate)</v>
+        <f t="shared" si="0"/>
+        <v>number (0)</v>
       </c>
       <c r="D3" s="5" t="str">
-        <f>INDEX(fleet_cols_types, MATCH(D2, fleet_cols_names, 0)) &amp; IF("Required" = INDEX(fleet_cols_required, MATCH(D2, fleet_cols_names, 0)), "*", " (" &amp; INDEX(fleet_cols_default, MATCH(D2, fleet_cols_names, 0)) &amp; ")")</f>
-        <v>(recalculate)</v>
+        <f t="shared" si="0"/>
+        <v>string*</v>
       </c>
       <c r="E3" s="5" t="str">
-        <f>INDEX(fleet_cols_types, MATCH(E2, fleet_cols_names, 0)) &amp; IF("Required" = INDEX(fleet_cols_required, MATCH(E2, fleet_cols_names, 0)), "*", " (" &amp; INDEX(fleet_cols_default, MATCH(E2, fleet_cols_names, 0)) &amp; ")")</f>
-        <v>(recalculate)</v>
+        <f t="shared" si="0"/>
+        <v>string*</v>
       </c>
       <c r="F3" s="5" t="str">
-        <f>INDEX(fleet_cols_types, MATCH(F2, fleet_cols_names, 0)) &amp; IF("Required" = INDEX(fleet_cols_required, MATCH(F2, fleet_cols_names, 0)), "*", " (" &amp; INDEX(fleet_cols_default, MATCH(F2, fleet_cols_names, 0)) &amp; ")")</f>
-        <v>(recalculate)</v>
+        <f t="shared" si="0"/>
+        <v>string*</v>
       </c>
       <c r="G3" s="5" t="str">
-        <f>INDEX(fleet_cols_types, MATCH(G2, fleet_cols_names, 0)) &amp; IF("Required" = INDEX(fleet_cols_required, MATCH(G2, fleet_cols_names, 0)), "*", " (" &amp; INDEX(fleet_cols_default, MATCH(G2, fleet_cols_names, 0)) &amp; ")")</f>
-        <v>(recalculate)</v>
+        <f t="shared" si="0"/>
+        <v>boolean (FALSE)</v>
       </c>
       <c r="H3" s="5" t="str">
-        <f>INDEX(fleet_cols_types, MATCH(H2, fleet_cols_names, 0)) &amp; IF("Required" = INDEX(fleet_cols_required, MATCH(H2, fleet_cols_names, 0)), "*", " (" &amp; INDEX(fleet_cols_default, MATCH(H2, fleet_cols_names, 0)) &amp; ")")</f>
-        <v>(recalculate)</v>
+        <f t="shared" si="0"/>
+        <v>number (0)</v>
       </c>
       <c r="I3" s="5" t="str">
-        <f>INDEX(fleet_cols_types, MATCH(I2, fleet_cols_names, 0)) &amp; IF("Required" = INDEX(fleet_cols_required, MATCH(I2, fleet_cols_names, 0)), "*", " (" &amp; INDEX(fleet_cols_default, MATCH(I2, fleet_cols_names, 0)) &amp; ")")</f>
-        <v>(recalculate)</v>
+        <f t="shared" si="0"/>
+        <v>number (1000)</v>
       </c>
       <c r="J3" s="5" t="str">
-        <f>INDEX(fleet_cols_types, MATCH(J2, fleet_cols_names, 0)) &amp; IF("Required" = INDEX(fleet_cols_required, MATCH(J2, fleet_cols_names, 0)), "*", " (" &amp; INDEX(fleet_cols_default, MATCH(J2, fleet_cols_names, 0)) &amp; ")")</f>
-        <v>(recalculate)</v>
+        <f t="shared" si="0"/>
+        <v>number (10)</v>
       </c>
       <c r="K3" s="5" t="str">
-        <f>INDEX(fleet_cols_types, MATCH(K2, fleet_cols_names, 0)) &amp; IF("Required" = INDEX(fleet_cols_required, MATCH(K2, fleet_cols_names, 0)), "*", " (" &amp; INDEX(fleet_cols_default, MATCH(K2, fleet_cols_names, 0)) &amp; ")")</f>
-        <v>(recalculate)</v>
-      </c>
-    </row>
-    <row r="4" ht="20" customHeight="1" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>number (15)</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="str">
-        <f>HYPERLINK("#fleet." &amp; A2, "help")</f>
-        <v>(recalculate)</v>
+        <f t="shared" ref="A4:K4" si="1">HYPERLINK("#fleet." &amp; A2, "help")</f>
+        <v>help</v>
       </c>
       <c r="B4" s="7" t="str">
-        <f>HYPERLINK("#fleet." &amp; B2, "help")</f>
-        <v>(recalculate)</v>
+        <f t="shared" si="1"/>
+        <v>help</v>
       </c>
       <c r="C4" s="7" t="str">
-        <f>HYPERLINK("#fleet." &amp; C2, "help")</f>
-        <v>(recalculate)</v>
+        <f t="shared" si="1"/>
+        <v>help</v>
       </c>
       <c r="D4" s="7" t="str">
-        <f>HYPERLINK("#fleet." &amp; D2, "help")</f>
-        <v>(recalculate)</v>
+        <f t="shared" si="1"/>
+        <v>help</v>
       </c>
       <c r="E4" s="7" t="str">
-        <f>HYPERLINK("#fleet." &amp; E2, "help")</f>
-        <v>(recalculate)</v>
+        <f t="shared" si="1"/>
+        <v>help</v>
       </c>
       <c r="F4" s="7" t="str">
-        <f>HYPERLINK("#fleet." &amp; F2, "help")</f>
-        <v>(recalculate)</v>
+        <f t="shared" si="1"/>
+        <v>help</v>
       </c>
       <c r="G4" s="7" t="str">
-        <f>HYPERLINK("#fleet." &amp; G2, "help")</f>
-        <v>(recalculate)</v>
+        <f t="shared" si="1"/>
+        <v>help</v>
       </c>
       <c r="H4" s="7" t="str">
-        <f>HYPERLINK("#fleet." &amp; H2, "help")</f>
-        <v>(recalculate)</v>
+        <f t="shared" si="1"/>
+        <v>help</v>
       </c>
       <c r="I4" s="7" t="str">
-        <f>HYPERLINK("#fleet." &amp; I2, "help")</f>
-        <v>(recalculate)</v>
+        <f t="shared" si="1"/>
+        <v>help</v>
       </c>
       <c r="J4" s="7" t="str">
-        <f>HYPERLINK("#fleet." &amp; J2, "help")</f>
-        <v>(recalculate)</v>
+        <f t="shared" si="1"/>
+        <v>help</v>
       </c>
       <c r="K4" s="7" t="str">
-        <f>HYPERLINK("#fleet." &amp; K2, "help")</f>
-        <v>(recalculate)</v>
-      </c>
-    </row>
-    <row r="5" ht="25" customHeight="1" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>help</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>103</v>
       </c>
@@ -8289,7 +8332,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" ht="25" customHeight="1" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>103</v>
       </c>
@@ -8324,7 +8367,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" ht="25" customHeight="1" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>107</v>
       </c>
@@ -8359,7 +8402,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" ht="25" customHeight="1" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>107</v>
       </c>
@@ -8394,7 +8437,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" ht="25" customHeight="1" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>108</v>
       </c>
@@ -8429,7 +8472,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" ht="25" customHeight="1" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>109</v>
       </c>
@@ -8464,7 +8507,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" ht="25" customHeight="1" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>110</v>
       </c>
@@ -8499,7 +8542,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" ht="25" customHeight="1" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>111</v>
       </c>
@@ -8541,7 +8584,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
 
@@ -8551,17 +8594,17 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18" style="1" customWidth="1"/>
     <col min="2" max="3" width="22" style="1" customWidth="1"/>
     <col min="4" max="4" width="19" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="25" customHeight="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>112</v>
       </c>
@@ -8575,7 +8618,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" ht="25" customHeight="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="2" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>116</v>
       </c>
@@ -8589,43 +8632,43 @@
         <v>119</v>
       </c>
     </row>
-    <row r="3" ht="12.5" customHeight="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" s="4" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="str">
         <f>INDEX(options_cols_types, MATCH(A2, options_cols_names, 0)) &amp; IF("Required" = INDEX(options_cols_required, MATCH(A2, options_cols_names, 0)), "*", " (" &amp; INDEX(options_cols_default, MATCH(A2, options_cols_names, 0)) &amp; ")")</f>
-        <v>(recalculate)</v>
+        <v>string*</v>
       </c>
       <c r="B3" s="5" t="str">
         <f>INDEX(options_cols_types, MATCH(B2, options_cols_names, 0)) &amp; IF("Required" = INDEX(options_cols_required, MATCH(B2, options_cols_names, 0)), "*", " (" &amp; INDEX(options_cols_default, MATCH(B2, options_cols_names, 0)) &amp; ")")</f>
-        <v>(recalculate)</v>
+        <v>string (UTC)</v>
       </c>
       <c r="C3" s="5" t="str">
         <f>INDEX(options_cols_types, MATCH(C2, options_cols_names, 0)) &amp; IF("Required" = INDEX(options_cols_required, MATCH(C2, options_cols_names, 0)), "*", " (" &amp; INDEX(options_cols_default, MATCH(C2, options_cols_names, 0)) &amp; ")")</f>
-        <v>(recalculate)</v>
+        <v>string (normal)</v>
       </c>
       <c r="D3" s="5" t="str">
         <f>INDEX(options_cols_types, MATCH(D2, options_cols_names, 0)) &amp; IF("Required" = INDEX(options_cols_required, MATCH(D2, options_cols_names, 0)), "*", " (" &amp; INDEX(options_cols_default, MATCH(D2, options_cols_names, 0)) &amp; ")")</f>
-        <v>(recalculate)</v>
-      </c>
-    </row>
-    <row r="4" ht="20" customHeight="1" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <v>string (osrm)</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="str">
         <f>HYPERLINK("#options." &amp; A2, "help")</f>
-        <v>(recalculate)</v>
+        <v>help</v>
       </c>
       <c r="B4" s="7" t="str">
         <f>HYPERLINK("#options." &amp; B2, "help")</f>
-        <v>(recalculate)</v>
+        <v>help</v>
       </c>
       <c r="C4" s="7" t="str">
         <f>HYPERLINK("#options." &amp; C2, "help")</f>
-        <v>(recalculate)</v>
+        <v>help</v>
       </c>
       <c r="D4" s="7" t="str">
         <f>HYPERLINK("#options." &amp; D2, "help")</f>
-        <v>(recalculate)</v>
-      </c>
-    </row>
-    <row r="5" ht="25" customHeight="1" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>help</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="8" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>120</v>
       </c>
@@ -8646,7 +8689,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
 
@@ -8656,10 +8699,10 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30" style="1" customWidth="1"/>
     <col min="2" max="2" width="20" style="1" customWidth="1"/>
@@ -8668,20 +8711,18 @@
     <col min="5" max="5" width="41" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>124</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C1" s="1"/>
       <c r="D1" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" ht="25" customHeight="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" s="2" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>127</v>
       </c>
@@ -8698,48 +8739,48 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" ht="12.5" customHeight="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="4" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="str">
         <f>INDEX(constraints_cols_types, MATCH(A2, constraints_cols_names, 0)) &amp; IF("Required" = INDEX(constraints_cols_required, MATCH(A2, constraints_cols_names, 0)), "*", " (" &amp; INDEX(constraints_cols_default, MATCH(A2, constraints_cols_names, 0)) &amp; ")")</f>
-        <v>(recalculate)</v>
+        <v>array of array of string ()</v>
       </c>
       <c r="B3" s="5" t="str">
         <f>INDEX(constraints_cols_types, MATCH(B2, constraints_cols_names, 0)) &amp; IF("Required" = INDEX(constraints_cols_required, MATCH(B2, constraints_cols_names, 0)), "*", " (" &amp; INDEX(constraints_cols_default, MATCH(B2, constraints_cols_names, 0)) &amp; ")")</f>
-        <v>(recalculate)</v>
+        <v>string*</v>
       </c>
       <c r="C3" s="5" t="str">
         <f>INDEX(constraints_cols_types, MATCH(C2, constraints_cols_names, 0)) &amp; IF("Required" = INDEX(constraints_cols_required, MATCH(C2, constraints_cols_names, 0)), "*", " (" &amp; INDEX(constraints_cols_default, MATCH(C2, constraints_cols_names, 0)) &amp; ")")</f>
-        <v>(recalculate)</v>
+        <v>number (3)</v>
       </c>
       <c r="D3" s="5" t="str">
         <f>INDEX(constraints_cols_types, MATCH(D2, constraints_cols_names, 0)) &amp; IF("Required" = INDEX(constraints_cols_required, MATCH(D2, constraints_cols_names, 0)), "*", " (" &amp; INDEX(constraints_cols_default, MATCH(D2, constraints_cols_names, 0)) &amp; ")")</f>
-        <v>(recalculate)</v>
+        <v>string*</v>
       </c>
       <c r="E3" s="5" t="str">
         <f>INDEX(constraints_cols_types, MATCH(E2, constraints_cols_names, 0)) &amp; IF("Required" = INDEX(constraints_cols_required, MATCH(E2, constraints_cols_names, 0)), "*", " (" &amp; INDEX(constraints_cols_default, MATCH(E2, constraints_cols_names, 0)) &amp; ")")</f>
-        <v>(recalculate)</v>
-      </c>
-    </row>
-    <row r="4" ht="20" customHeight="1" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <v>number (10)</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="str">
         <f>HYPERLINK("#constraints." &amp; A2, "help")</f>
-        <v>(recalculate)</v>
+        <v>help</v>
       </c>
       <c r="B4" s="7" t="str">
         <f>HYPERLINK("#constraints." &amp; B2, "help")</f>
-        <v>(recalculate)</v>
+        <v>help</v>
       </c>
       <c r="C4" s="7" t="str">
         <f>HYPERLINK("#constraints." &amp; C2, "help")</f>
-        <v>(recalculate)</v>
+        <v>help</v>
       </c>
       <c r="D4" s="7" t="str">
         <f>HYPERLINK("#constraints." &amp; D2, "help")</f>
-        <v>(recalculate)</v>
+        <v>help</v>
       </c>
       <c r="E4" s="7" t="str">
         <f>HYPERLINK("#constraints." &amp; E2, "help")</f>
-        <v>(recalculate)</v>
+        <v>help</v>
       </c>
     </row>
   </sheetData>
@@ -8749,20 +8790,20 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" style="9" customWidth="1"/>
     <col min="2" max="2" width="50" style="9" customWidth="1"/>
@@ -8772,7 +8813,7 @@
     <col min="6" max="6" width="64" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="25" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>132</v>
       </c>
@@ -8792,7 +8833,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="10" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B2" s="10" t="s">
         <v>4</v>
       </c>
@@ -8809,7 +8850,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="3" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="10" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="B3" s="10" t="s">
         <v>10</v>
       </c>
@@ -8826,7 +8867,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" s="9" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>144</v>
       </c>
@@ -8842,7 +8883,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="5" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" s="10" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="B5" s="10" t="s">
         <v>146</v>
       </c>
@@ -8859,7 +8900,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" s="9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>148</v>
       </c>
@@ -8875,7 +8916,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="7" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" s="10" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B7" s="10" t="s">
         <v>5</v>
       </c>
@@ -8892,7 +8933,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="8" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" s="10" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B8" s="10" t="s">
         <v>6</v>
       </c>
@@ -8909,7 +8950,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" s="9" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>152</v>
       </c>
@@ -8925,7 +8966,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" s="9" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>155</v>
       </c>
@@ -8941,7 +8982,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="11" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" s="10" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="B11" s="10" t="s">
         <v>157</v>
       </c>
@@ -8958,7 +8999,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="12" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" s="10" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B12" s="10" t="s">
         <v>159</v>
       </c>
@@ -8975,7 +9016,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="13" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" s="10" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B13" s="10" t="s">
         <v>161</v>
       </c>
@@ -8992,7 +9033,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" s="9" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
         <v>163</v>
       </c>
@@ -9008,7 +9049,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="15" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" s="10" customFormat="1" ht="208" x14ac:dyDescent="0.2">
       <c r="B15" s="10" t="s">
         <v>8</v>
       </c>
@@ -9025,7 +9066,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="16" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" s="10" customFormat="1" ht="208" x14ac:dyDescent="0.2">
       <c r="B16" s="10" t="s">
         <v>7</v>
       </c>
@@ -9042,7 +9083,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="17" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" s="10" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="B17" s="10" t="s">
         <v>9</v>
       </c>
@@ -9059,7 +9100,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" s="9" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>169</v>
       </c>
@@ -9075,7 +9116,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="19" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" s="10" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B19" s="10" t="s">
         <v>171</v>
       </c>
@@ -9092,7 +9133,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="20" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" s="10" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B20" s="10" t="s">
         <v>173</v>
       </c>
@@ -9109,7 +9150,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="21" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" s="10" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B21" s="10" t="s">
         <v>175</v>
       </c>
@@ -9128,8 +9169,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -9139,10 +9180,10 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" style="9" customWidth="1"/>
     <col min="2" max="2" width="50" style="9" customWidth="1"/>
@@ -9152,7 +9193,7 @@
     <col min="6" max="6" width="64" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="25" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>132</v>
       </c>
@@ -9172,7 +9213,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="10" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B2" s="10" t="s">
         <v>4</v>
       </c>
@@ -9189,7 +9230,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="3" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="10" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B3" s="10" t="s">
         <v>177</v>
       </c>
@@ -9206,7 +9247,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="4" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" s="10" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="B4" s="10" t="s">
         <v>10</v>
       </c>
@@ -9223,7 +9264,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="5" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" s="10" customFormat="1" ht="160" x14ac:dyDescent="0.2">
       <c r="B5" s="10" t="s">
         <v>21</v>
       </c>
@@ -9240,7 +9281,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="6" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" s="10" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="B6" s="10" t="s">
         <v>181</v>
       </c>
@@ -9257,7 +9298,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="7" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" s="10" customFormat="1" ht="160" x14ac:dyDescent="0.2">
       <c r="B7" s="10" t="s">
         <v>183</v>
       </c>
@@ -9274,7 +9315,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="8" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" s="10" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="B8" s="10" t="s">
         <v>185</v>
       </c>
@@ -9291,7 +9332,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="9" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" s="10" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="B9" s="10" t="s">
         <v>188</v>
       </c>
@@ -9308,7 +9349,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="10" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" s="10" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B10" s="10" t="s">
         <v>23</v>
       </c>
@@ -9325,7 +9366,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" s="9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>191</v>
       </c>
@@ -9341,7 +9382,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="12" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" s="10" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B12" s="10" t="s">
         <v>193</v>
       </c>
@@ -9358,7 +9399,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="13" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" s="10" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="B13" s="10" t="s">
         <v>195</v>
       </c>
@@ -9375,7 +9416,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="14" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" s="10" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="B14" s="10" t="s">
         <v>197</v>
       </c>
@@ -9392,7 +9433,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="15" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" s="10" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="B15" s="10" t="s">
         <v>22</v>
       </c>
@@ -9409,7 +9450,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" s="9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>148</v>
       </c>
@@ -9425,7 +9466,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="17" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" s="10" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B17" s="10" t="s">
         <v>5</v>
       </c>
@@ -9442,7 +9483,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="18" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" s="10" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B18" s="10" t="s">
         <v>6</v>
       </c>
@@ -9459,7 +9500,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" s="9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>163</v>
       </c>
@@ -9475,7 +9516,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="20" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" s="10" customFormat="1" ht="208" x14ac:dyDescent="0.2">
       <c r="B20" s="10" t="s">
         <v>8</v>
       </c>
@@ -9492,7 +9533,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="21" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" s="10" customFormat="1" ht="208" x14ac:dyDescent="0.2">
       <c r="B21" s="10" t="s">
         <v>7</v>
       </c>
@@ -9509,7 +9550,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="22" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" s="10" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="B22" s="10" t="s">
         <v>9</v>
       </c>
@@ -9526,7 +9567,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" s="9" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
         <v>169</v>
       </c>
@@ -9542,7 +9583,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="24" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" s="10" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B24" s="10" t="s">
         <v>171</v>
       </c>
@@ -9559,7 +9600,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="25" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" s="10" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B25" s="10" t="s">
         <v>173</v>
       </c>
@@ -9576,7 +9617,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="26" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" s="10" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B26" s="10" t="s">
         <v>175</v>
       </c>
@@ -9595,20 +9636,20 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" style="9" customWidth="1"/>
     <col min="2" max="2" width="50" style="9" customWidth="1"/>
@@ -9618,7 +9659,7 @@
     <col min="6" max="6" width="64" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="25" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>132</v>
       </c>
@@ -9638,7 +9679,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="10" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B2" s="10" t="s">
         <v>4</v>
       </c>
@@ -9655,7 +9696,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="3" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="10" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="B3" s="10" t="s">
         <v>202</v>
       </c>
@@ -9672,7 +9713,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="4" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" s="10" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="B4" s="10" t="s">
         <v>93</v>
       </c>
@@ -9689,7 +9730,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="5" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" s="10" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="B5" s="10" t="s">
         <v>205</v>
       </c>
@@ -9706,7 +9747,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="6" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" s="10" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="B6" s="10" t="s">
         <v>207</v>
       </c>
@@ -9723,7 +9764,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" s="9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>209</v>
       </c>
@@ -9739,7 +9780,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="8" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" s="10" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="B8" s="10" t="s">
         <v>211</v>
       </c>
@@ -9756,7 +9797,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="9" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" s="10" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="B9" s="10" t="s">
         <v>212</v>
       </c>
@@ -9773,7 +9814,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="10" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" s="10" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="B10" s="10" t="s">
         <v>94</v>
       </c>
@@ -9790,7 +9831,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" s="9" customFormat="1" ht="160" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>213</v>
       </c>
@@ -9806,7 +9847,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="12" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" s="10" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="B12" s="10" t="s">
         <v>100</v>
       </c>
@@ -9823,7 +9864,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="13" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" s="10" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B13" s="10" t="s">
         <v>101</v>
       </c>
@@ -9840,7 +9881,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="14" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" s="10" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B14" s="10" t="s">
         <v>102</v>
       </c>
@@ -9857,7 +9898,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="15" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" s="10" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="B15" s="10" t="s">
         <v>218</v>
       </c>
@@ -9874,7 +9915,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="16" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" s="10" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B16" s="10" t="s">
         <v>220</v>
       </c>
@@ -9891,7 +9932,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" s="9" customFormat="1" ht="160" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>222</v>
       </c>
@@ -9907,7 +9948,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="18" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" s="10" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B18" s="10" t="s">
         <v>224</v>
       </c>
@@ -9924,7 +9965,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="19" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" s="10" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B19" s="10" t="s">
         <v>226</v>
       </c>
@@ -9941,7 +9982,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" s="9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
         <v>228</v>
       </c>
@@ -9957,7 +9998,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="21" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" s="10" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="B21" s="10" t="s">
         <v>230</v>
       </c>
@@ -9974,7 +10015,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="22" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" s="10" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="B22" s="10" t="s">
         <v>231</v>
       </c>
@@ -9991,7 +10032,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="23" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" s="10" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="B23" s="10" t="s">
         <v>232</v>
       </c>
@@ -10008,7 +10049,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" s="9" customFormat="1" ht="224" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
         <v>233</v>
       </c>
@@ -10024,7 +10065,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="25" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" s="10" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B25" s="10" t="s">
         <v>95</v>
       </c>
@@ -10041,7 +10082,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="26" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" s="10" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="B26" s="10" t="s">
         <v>236</v>
       </c>
@@ -10058,7 +10099,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="27" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" s="10" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="B27" s="10" t="s">
         <v>99</v>
       </c>
@@ -10075,7 +10116,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="28" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" s="10" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="B28" s="10" t="s">
         <v>239</v>
       </c>
@@ -10092,7 +10133,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" s="9" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
         <v>241</v>
       </c>
@@ -10108,7 +10149,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="30" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" s="10" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B30" s="10" t="s">
         <v>243</v>
       </c>
@@ -10125,7 +10166,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" s="9" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>245</v>
       </c>
@@ -10141,7 +10182,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="32" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" s="10" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B32" s="10" t="s">
         <v>247</v>
       </c>
@@ -10158,7 +10199,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="33" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" s="10" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B33" s="10" t="s">
         <v>249</v>
       </c>
@@ -10175,7 +10216,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" s="9" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
         <v>251</v>
       </c>
@@ -10191,7 +10232,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="35" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" s="10" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B35" s="10" t="s">
         <v>253</v>
       </c>
@@ -10208,7 +10249,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" s="9" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A36" s="12" t="s">
         <v>255</v>
       </c>
@@ -10224,7 +10265,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="37" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" s="10" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B37" s="10" t="s">
         <v>257</v>
       </c>
@@ -10241,7 +10282,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="38" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" s="10" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B38" s="10" t="s">
         <v>258</v>
       </c>
@@ -10258,7 +10299,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" s="9" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="A39" s="12" t="s">
         <v>260</v>
       </c>
@@ -10274,7 +10315,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="40" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" s="10" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B40" s="10" t="s">
         <v>262</v>
       </c>
@@ -10291,7 +10332,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="41" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" s="10" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B41" s="10" t="s">
         <v>264</v>
       </c>
@@ -10308,7 +10349,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" s="9" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A42" s="12" t="s">
         <v>265</v>
       </c>
@@ -10324,7 +10365,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="43" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" s="10" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="B43" s="10" t="s">
         <v>267</v>
       </c>
@@ -10341,7 +10382,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" s="9" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A44" s="12" t="s">
         <v>269</v>
       </c>
@@ -10357,7 +10398,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="45" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" s="10" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B45" s="10" t="s">
         <v>271</v>
       </c>
@@ -10374,7 +10415,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="46" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" s="10" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B46" s="10" t="s">
         <v>272</v>
       </c>
@@ -10391,7 +10432,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="47" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" s="9" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A47" s="12" t="s">
         <v>274</v>
       </c>
@@ -10407,7 +10448,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="48" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" s="10" customFormat="1" ht="208" x14ac:dyDescent="0.2">
       <c r="B48" s="10" t="s">
         <v>97</v>
       </c>
@@ -10424,7 +10465,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="49" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:6" s="10" customFormat="1" ht="208" x14ac:dyDescent="0.2">
       <c r="B49" s="10" t="s">
         <v>96</v>
       </c>
@@ -10441,7 +10482,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="50" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:6" s="10" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="B50" s="10" t="s">
         <v>98</v>
       </c>
@@ -10460,8 +10501,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -10471,10 +10512,10 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" style="9" customWidth="1"/>
     <col min="2" max="2" width="50" style="9" customWidth="1"/>
@@ -10484,7 +10525,7 @@
     <col min="6" max="6" width="64" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="25" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>132</v>
       </c>
@@ -10504,7 +10545,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="10" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="B2" s="10" t="s">
         <v>116</v>
       </c>
@@ -10521,7 +10562,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="3" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="10" customFormat="1" ht="176" x14ac:dyDescent="0.2">
       <c r="B3" s="10" t="s">
         <v>119</v>
       </c>
@@ -10538,7 +10579,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="4" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" s="10" customFormat="1" ht="176" x14ac:dyDescent="0.2">
       <c r="B4" s="10" t="s">
         <v>118</v>
       </c>
@@ -10555,7 +10596,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="5" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" s="10" customFormat="1" ht="160" x14ac:dyDescent="0.2">
       <c r="B5" s="10" t="s">
         <v>117</v>
       </c>
@@ -10574,6 +10615,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>